<commit_message>
fixing the date format issue
</commit_message>
<xml_diff>
--- a/Movie.xlsx
+++ b/Movie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>